<commit_message>
Update volume table for accuracy.
</commit_message>
<xml_diff>
--- a/tabella dei volumi.xlsx
+++ b/tabella dei volumi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ezmirondeniku/Desktop/elaborato-database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411F8555-BE41-1945-80AA-8AD2A1AC760A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF92D20C-4D4B-6248-918D-CB763F4CBE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{43723271-4DD4-433C-9C4E-C013E360E198}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="121">
   <si>
     <t>concetto</t>
   </si>
@@ -273,18 +273,9 @@
     <t>10S</t>
   </si>
   <si>
-    <t>5L</t>
-  </si>
-  <si>
-    <t>2L</t>
-  </si>
-  <si>
     <t>20S</t>
   </si>
   <si>
-    <t>13L</t>
-  </si>
-  <si>
     <t>Op9</t>
   </si>
   <si>
@@ -306,21 +297,12 @@
     <t>=</t>
   </si>
   <si>
-    <t>12000/gg</t>
-  </si>
-  <si>
     <t>50/gg</t>
   </si>
   <si>
-    <t>1250/gg</t>
-  </si>
-  <si>
     <t>60/gg</t>
   </si>
   <si>
-    <t>1020/gg</t>
-  </si>
-  <si>
     <t>1080/gg</t>
   </si>
   <si>
@@ -333,17 +315,98 @@
     <t>200/gg</t>
   </si>
   <si>
-    <t>10400/gg</t>
-  </si>
-  <si>
     <t>10600/gg</t>
+  </si>
+  <si>
+    <t>80/m</t>
+  </si>
+  <si>
+    <t>160/m</t>
+  </si>
+  <si>
+    <t>1L</t>
+  </si>
+  <si>
+    <t>1/gg</t>
+  </si>
+  <si>
+    <t>40L</t>
+  </si>
+  <si>
+    <t>40/gg</t>
+  </si>
+  <si>
+    <t>STIPENDIO</t>
+  </si>
+  <si>
+    <t>PERCEPISCE</t>
+  </si>
+  <si>
+    <t>Op10a</t>
+  </si>
+  <si>
+    <t>PAGA</t>
+  </si>
+  <si>
+    <t>10000S</t>
+  </si>
+  <si>
+    <t>2000L</t>
+  </si>
+  <si>
+    <t>1/M</t>
+  </si>
+  <si>
+    <t>Op10b</t>
+  </si>
+  <si>
+    <t>Calcolo stipendio dipendenti(meccanico)</t>
+  </si>
+  <si>
+    <t>Calcolo stipendio dipendenti(consulente)</t>
+  </si>
+  <si>
+    <t>CONSULENTI</t>
+  </si>
+  <si>
+    <t>50000S</t>
+  </si>
+  <si>
+    <t>7L</t>
+  </si>
+  <si>
+    <t>12500/gg</t>
+  </si>
+  <si>
+    <t>1300/gg</t>
+  </si>
+  <si>
+    <t>4L</t>
+  </si>
+  <si>
+    <t>1140/gg</t>
+  </si>
+  <si>
+    <t>15L</t>
+  </si>
+  <si>
+    <t>10800/gg</t>
+  </si>
+  <si>
+    <t>4000L</t>
+  </si>
+  <si>
+    <t>24000/m</t>
+  </si>
+  <si>
+    <t>12000/m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +440,13 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -423,8 +493,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1039,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7CF6F4-9A21-6746-81DA-F55FEE7F3A9F}">
-  <dimension ref="A1:N134"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1070,7 +1140,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" t="s">
@@ -1136,18 +1206,18 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>41</v>
@@ -1155,91 +1225,91 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
       <c r="D10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
         <v>85</v>
       </c>
-      <c r="F11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1250,10 +1320,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1264,10 +1334,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1278,130 +1348,130 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>41</v>
+      <c r="B23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
       </c>
       <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
         <v>5</v>
       </c>
-      <c r="D24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" t="s">
-        <v>86</v>
+      <c r="D25" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>77</v>
       </c>
-      <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26">
-        <v>25</v>
-      </c>
-      <c r="E26" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
@@ -1410,12 +1480,12 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
@@ -1429,7 +1499,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
@@ -1438,12 +1508,12 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>26</v>
@@ -1456,22 +1526,22 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="A39" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
         <v>25</v>
@@ -1485,7 +1555,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
         <v>26</v>
@@ -1499,7 +1569,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
         <v>25</v>
@@ -1511,107 +1581,107 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E43" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" t="s">
-        <v>86</v>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>59</v>
       </c>
-      <c r="B44" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47">
+        <v>18</v>
+      </c>
+      <c r="E47" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47" t="s">
         <v>88</v>
       </c>
-      <c r="D44">
-        <v>17</v>
-      </c>
-      <c r="E44" t="s">
-        <v>92</v>
-      </c>
-      <c r="F44" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B50" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B52" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D52" s="5" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" t="s">
-        <v>26</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1622,10 +1692,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1636,10 +1706,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1650,38 +1720,38 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="7">
+        <v>1</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1692,130 +1762,130 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E60" t="s">
-        <v>85</v>
-      </c>
-      <c r="F60" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B61" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>56</v>
+      </c>
+      <c r="B63" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E64" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>45</v>
       </c>
-      <c r="B61" t="s">
-        <v>79</v>
-      </c>
-      <c r="C61" t="s">
-        <v>88</v>
-      </c>
-      <c r="D61">
-        <v>18</v>
-      </c>
-      <c r="E61" t="s">
-        <v>92</v>
-      </c>
-      <c r="F61" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="B65" t="s">
+        <v>60</v>
+      </c>
+      <c r="C65" t="s">
+        <v>85</v>
+      </c>
+      <c r="D65">
+        <v>19</v>
+      </c>
+      <c r="E65" t="s">
+        <v>87</v>
+      </c>
+      <c r="F65" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B64" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
+      <c r="B68" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B70" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D70" s="5" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B67" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>34</v>
-      </c>
-      <c r="B68" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="D68" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>35</v>
-      </c>
-      <c r="B69" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-      <c r="D69" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>36</v>
-      </c>
-      <c r="B70" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-      <c r="D70" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B71" t="s">
         <v>25</v>
@@ -1829,13 +1899,13 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="B72" t="s">
         <v>26</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D72" t="s">
         <v>41</v>
@@ -1843,13 +1913,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="B73" t="s">
         <v>25</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73" t="s">
         <v>42</v>
@@ -1857,35 +1927,35 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D74" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>65</v>
-      </c>
-      <c r="B75" t="s">
-        <v>26</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
-      <c r="D75" t="s">
-        <v>41</v>
+      <c r="A75" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" s="7">
+        <v>1</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B76" t="s">
         <v>25</v>
@@ -1894,18 +1964,18 @@
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B77" t="s">
         <v>26</v>
       </c>
       <c r="C77">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
         <v>41</v>
@@ -1913,658 +1983,1130 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B78" t="s">
         <v>25</v>
       </c>
       <c r="C78">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E79" t="s">
-        <v>85</v>
-      </c>
-      <c r="F79" t="s">
-        <v>86</v>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>64</v>
+      </c>
+      <c r="B79" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>65</v>
+      </c>
+      <c r="B80" t="s">
+        <v>26</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>56</v>
+      </c>
+      <c r="B81" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" t="s">
+        <v>26</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+      <c r="D82" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="D83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" t="s">
+        <v>82</v>
+      </c>
+      <c r="F84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B85" t="s">
+        <v>116</v>
+      </c>
+      <c r="C85" t="s">
+        <v>85</v>
+      </c>
+      <c r="D85">
+        <v>53</v>
+      </c>
+      <c r="E85" t="s">
+        <v>91</v>
+      </c>
+      <c r="F85" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>62</v>
+      </c>
+      <c r="B91" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>34</v>
+      </c>
+      <c r="B92" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>35</v>
+      </c>
+      <c r="B93" t="s">
+        <v>25</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>36</v>
+      </c>
+      <c r="B94" t="s">
+        <v>26</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95" s="7">
+        <v>1</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>37</v>
+      </c>
+      <c r="B96" t="s">
+        <v>25</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>63</v>
+      </c>
+      <c r="B97" t="s">
+        <v>26</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>64</v>
+      </c>
+      <c r="B98" t="s">
+        <v>25</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>64</v>
+      </c>
+      <c r="B99" t="s">
+        <v>25</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B100" t="s">
+        <v>26</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>56</v>
+      </c>
+      <c r="B101" t="s">
+        <v>25</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>66</v>
+      </c>
+      <c r="B102" t="s">
+        <v>26</v>
+      </c>
+      <c r="C102">
+        <v>10</v>
+      </c>
+      <c r="D102" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>67</v>
+      </c>
+      <c r="B103" t="s">
+        <v>25</v>
+      </c>
+      <c r="C103">
+        <v>10</v>
+      </c>
+      <c r="D103" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A104" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E104" t="s">
+        <v>82</v>
+      </c>
+      <c r="F104" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>78</v>
+      </c>
+      <c r="B105" t="s">
         <v>75</v>
       </c>
-      <c r="C80" t="s">
-        <v>88</v>
-      </c>
-      <c r="D80">
-        <v>52</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="C105" t="s">
+        <v>85</v>
+      </c>
+      <c r="D105">
+        <v>54</v>
+      </c>
+      <c r="E105" t="s">
+        <v>91</v>
+      </c>
+      <c r="F105" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>69</v>
+      </c>
+      <c r="B107" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>71</v>
+      </c>
+      <c r="B109" t="s">
+        <v>25</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>72</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D111" s="7">
+        <v>2</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>73</v>
+      </c>
+      <c r="B114" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>37</v>
+      </c>
+      <c r="B116" t="s">
+        <v>25</v>
+      </c>
+      <c r="C116">
+        <v>40</v>
+      </c>
+      <c r="D116" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C117" s="7"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>97</v>
       </c>
-      <c r="F80" t="s">
+      <c r="C118" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D118" s="7">
+        <v>40</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F118" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B83" t="s">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>79</v>
+      </c>
+      <c r="B120" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>81</v>
+      </c>
+      <c r="B122" t="s">
+        <v>25</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C123" s="7"/>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>95</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D124" s="7">
+        <v>1</v>
+      </c>
+      <c r="E124" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
+      <c r="F124" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>101</v>
+      </c>
+      <c r="B126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B127" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C127" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D127" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>34</v>
-      </c>
-      <c r="B87" t="s">
-        <v>26</v>
-      </c>
-      <c r="C87">
-        <v>1</v>
-      </c>
-      <c r="D87" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>35</v>
-      </c>
-      <c r="B88" t="s">
-        <v>25</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-      <c r="D88" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>36</v>
-      </c>
-      <c r="B89" t="s">
-        <v>26</v>
-      </c>
-      <c r="C89">
-        <v>1</v>
-      </c>
-      <c r="D89" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>99</v>
+      </c>
+      <c r="B128" t="s">
+        <v>25</v>
+      </c>
+      <c r="C128">
+        <v>2000</v>
+      </c>
+      <c r="D128" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>100</v>
+      </c>
+      <c r="B129" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129">
+        <v>2000</v>
+      </c>
+      <c r="D129" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>64</v>
+      </c>
+      <c r="B130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C130">
+        <v>2000</v>
+      </c>
+      <c r="D130" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>64</v>
+      </c>
+      <c r="B131" t="s">
+        <v>25</v>
+      </c>
+      <c r="C131">
+        <v>2000</v>
+      </c>
+      <c r="D131" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>102</v>
+      </c>
+      <c r="B132" t="s">
+        <v>26</v>
+      </c>
+      <c r="C132">
+        <v>2000</v>
+      </c>
+      <c r="D132" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B90" t="s">
-        <v>25</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-      <c r="D90" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>63</v>
-      </c>
-      <c r="B91" t="s">
-        <v>26</v>
-      </c>
-      <c r="C91">
+      <c r="B133" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C133" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D133" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>37</v>
+      </c>
+      <c r="B134" t="s">
+        <v>25</v>
+      </c>
+      <c r="C134">
+        <v>2000</v>
+      </c>
+      <c r="D134" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A135" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C135" s="7"/>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>103</v>
+      </c>
+      <c r="B136" t="s">
+        <v>118</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D136" s="7">
+        <v>24000</v>
+      </c>
+      <c r="E136" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F136" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>106</v>
+      </c>
+      <c r="B138" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A139" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>99</v>
+      </c>
+      <c r="B140" t="s">
+        <v>25</v>
+      </c>
+      <c r="C140">
+        <v>1000</v>
+      </c>
+      <c r="D140" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>100</v>
+      </c>
+      <c r="B141" t="s">
+        <v>26</v>
+      </c>
+      <c r="C141">
+        <v>1000</v>
+      </c>
+      <c r="D141" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>109</v>
+      </c>
+      <c r="B142" t="s">
+        <v>25</v>
+      </c>
+      <c r="C142">
+        <v>1000</v>
+      </c>
+      <c r="D142" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>109</v>
+      </c>
+      <c r="B143" t="s">
+        <v>25</v>
+      </c>
+      <c r="C143">
+        <v>1000</v>
+      </c>
+      <c r="D143" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>102</v>
+      </c>
+      <c r="B144" t="s">
+        <v>26</v>
+      </c>
+      <c r="C144">
+        <v>1000</v>
+      </c>
+      <c r="D144" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C145" s="7">
+        <v>1000</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>37</v>
+      </c>
+      <c r="B146" t="s">
+        <v>25</v>
+      </c>
+      <c r="C146">
+        <v>1000</v>
+      </c>
+      <c r="D146" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A147" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C147" s="7"/>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F147" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>110</v>
+      </c>
+      <c r="B148" t="s">
+        <v>104</v>
+      </c>
+      <c r="C148" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D148" s="7">
+        <v>12000</v>
+      </c>
+      <c r="E148" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F148" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D91" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>64</v>
-      </c>
-      <c r="B92" t="s">
-        <v>25</v>
-      </c>
-      <c r="C92">
-        <v>2</v>
-      </c>
-      <c r="D92" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>64</v>
-      </c>
-      <c r="B93" t="s">
-        <v>25</v>
-      </c>
-      <c r="C93">
-        <v>2</v>
-      </c>
-      <c r="D93" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>65</v>
-      </c>
-      <c r="B94" t="s">
-        <v>26</v>
-      </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-      <c r="D94" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>56</v>
-      </c>
-      <c r="B95" t="s">
-        <v>25</v>
-      </c>
-      <c r="C95">
-        <v>1</v>
-      </c>
-      <c r="D95" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>66</v>
-      </c>
-      <c r="B96" t="s">
-        <v>26</v>
-      </c>
-      <c r="C96">
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B158" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158" t="s">
+        <v>25</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B159" t="s">
+        <v>4</v>
+      </c>
+      <c r="C159" t="s">
+        <v>25</v>
+      </c>
+      <c r="D159">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B160" t="s">
+        <v>5</v>
+      </c>
+      <c r="C160" t="s">
+        <v>26</v>
+      </c>
+      <c r="D160">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B161" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161" t="s">
+        <v>26</v>
+      </c>
+      <c r="D161" s="2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B162" t="s">
+        <v>7</v>
+      </c>
+      <c r="C162" t="s">
+        <v>26</v>
+      </c>
+      <c r="D162" s="2">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B163" t="s">
+        <v>8</v>
+      </c>
+      <c r="C163" t="s">
+        <v>25</v>
+      </c>
+      <c r="D163" s="2">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B164" t="s">
+        <v>9</v>
+      </c>
+      <c r="C164" t="s">
+        <v>26</v>
+      </c>
+      <c r="D164" s="2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B165" t="s">
         <v>10</v>
       </c>
-      <c r="D96" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>67</v>
-      </c>
-      <c r="B97" t="s">
-        <v>25</v>
-      </c>
-      <c r="C97">
-        <v>10</v>
-      </c>
-      <c r="D97" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E98" t="s">
-        <v>85</v>
-      </c>
-      <c r="F98" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>80</v>
-      </c>
-      <c r="B99" t="s">
-        <v>81</v>
-      </c>
-      <c r="C99" t="s">
-        <v>88</v>
-      </c>
-      <c r="D99">
-        <v>53</v>
-      </c>
-      <c r="E99" t="s">
-        <v>97</v>
-      </c>
-      <c r="F99" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>69</v>
-      </c>
-      <c r="B101" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A102" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>71</v>
-      </c>
-      <c r="B103" t="s">
-        <v>25</v>
-      </c>
-      <c r="C103">
-        <v>1</v>
-      </c>
-      <c r="D103" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="104" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C105" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>73</v>
-      </c>
-      <c r="B108" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>37</v>
-      </c>
-      <c r="B110" t="s">
-        <v>25</v>
-      </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
-      <c r="D110" t="s">
-        <v>42</v>
-      </c>
-      <c r="L110" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M110" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N110" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L111" t="s">
-        <v>3</v>
-      </c>
-      <c r="M111" t="s">
-        <v>25</v>
-      </c>
-      <c r="N111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L112" t="s">
-        <v>4</v>
-      </c>
-      <c r="M112" t="s">
-        <v>25</v>
-      </c>
-      <c r="N112">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>82</v>
-      </c>
-      <c r="B113" t="s">
-        <v>83</v>
-      </c>
-      <c r="L113" t="s">
-        <v>5</v>
-      </c>
-      <c r="M113" t="s">
-        <v>26</v>
-      </c>
-      <c r="N113">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="114" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C114" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D114" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L114" t="s">
-        <v>6</v>
-      </c>
-      <c r="M114" t="s">
-        <v>26</v>
-      </c>
-      <c r="N114" s="2">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>84</v>
-      </c>
-      <c r="B115" t="s">
-        <v>25</v>
-      </c>
-      <c r="C115">
-        <v>1</v>
-      </c>
-      <c r="D115" t="s">
-        <v>42</v>
-      </c>
-      <c r="L115" t="s">
-        <v>7</v>
-      </c>
-      <c r="M115" t="s">
-        <v>26</v>
-      </c>
-      <c r="N115" s="2">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L116" t="s">
-        <v>8</v>
-      </c>
-      <c r="M116" t="s">
-        <v>25</v>
-      </c>
-      <c r="N116" s="2">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L117" t="s">
-        <v>9</v>
-      </c>
-      <c r="M117" t="s">
-        <v>26</v>
-      </c>
-      <c r="N117" s="2">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L118" t="s">
-        <v>10</v>
-      </c>
-      <c r="M118" t="s">
-        <v>25</v>
-      </c>
-      <c r="N118" s="2">
+      <c r="C165" t="s">
+        <v>25</v>
+      </c>
+      <c r="D165" s="2">
         <v>100000</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L119" t="s">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B166" t="s">
         <v>11</v>
       </c>
-      <c r="M119" t="s">
-        <v>25</v>
-      </c>
-      <c r="N119" s="2">
+      <c r="C166" t="s">
+        <v>25</v>
+      </c>
+      <c r="D166" s="2">
         <v>500000</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L120" t="s">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B167" t="s">
         <v>27</v>
       </c>
-      <c r="M120" t="s">
-        <v>26</v>
-      </c>
-      <c r="N120" s="2">
+      <c r="C167" t="s">
+        <v>26</v>
+      </c>
+      <c r="D167" s="2">
         <v>2500000</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L121" t="s">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B168" t="s">
         <v>12</v>
       </c>
-      <c r="M121" t="s">
-        <v>25</v>
-      </c>
-      <c r="N121" s="2">
+      <c r="C168" t="s">
+        <v>25</v>
+      </c>
+      <c r="D168" s="2">
         <v>2500000</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L122" t="s">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B169" t="s">
         <v>13</v>
       </c>
-      <c r="M122" t="s">
-        <v>25</v>
-      </c>
-      <c r="N122" s="2">
+      <c r="C169" t="s">
+        <v>25</v>
+      </c>
+      <c r="D169" s="2">
         <v>100000</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L123" t="s">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B170" t="s">
         <v>14</v>
       </c>
-      <c r="M123" t="s">
-        <v>26</v>
-      </c>
-      <c r="N123" s="2">
+      <c r="C170" t="s">
+        <v>26</v>
+      </c>
+      <c r="D170" s="2">
         <v>100000</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L124" t="s">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B171" t="s">
         <v>15</v>
       </c>
-      <c r="M124" t="s">
-        <v>25</v>
-      </c>
-      <c r="N124" s="2">
+      <c r="C171" t="s">
+        <v>25</v>
+      </c>
+      <c r="D171" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L125" t="s">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B172" t="s">
         <v>16</v>
       </c>
-      <c r="M125" t="s">
-        <v>26</v>
-      </c>
-      <c r="N125" s="2">
+      <c r="C172" t="s">
+        <v>26</v>
+      </c>
+      <c r="D172" s="2">
         <v>150000</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L126" t="s">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B173" t="s">
         <v>17</v>
       </c>
-      <c r="M126" t="s">
-        <v>25</v>
-      </c>
-      <c r="N126" s="2">
+      <c r="C173" t="s">
+        <v>25</v>
+      </c>
+      <c r="D173" s="2">
         <v>150000</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L127" t="s">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B174" t="s">
         <v>18</v>
       </c>
-      <c r="M127" t="s">
-        <v>25</v>
-      </c>
-      <c r="N127">
+      <c r="C174" t="s">
+        <v>25</v>
+      </c>
+      <c r="D174">
         <v>2000</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="L128" t="s">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B175" t="s">
         <v>19</v>
       </c>
-      <c r="M128" t="s">
-        <v>26</v>
-      </c>
-      <c r="N128" s="2">
+      <c r="C175" t="s">
+        <v>26</v>
+      </c>
+      <c r="D175" s="2">
         <v>800000</v>
       </c>
     </row>
-    <row r="129" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L129" t="s">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B176" t="s">
         <v>20</v>
       </c>
-      <c r="M129" t="s">
-        <v>25</v>
-      </c>
-      <c r="N129" s="2">
+      <c r="C176" t="s">
+        <v>25</v>
+      </c>
+      <c r="D176" s="2">
         <v>400000</v>
       </c>
     </row>
-    <row r="130" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L130" t="s">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B177" t="s">
         <v>21</v>
       </c>
-      <c r="M130" t="s">
-        <v>26</v>
-      </c>
-      <c r="N130" s="2">
+      <c r="C177" t="s">
+        <v>26</v>
+      </c>
+      <c r="D177" s="2">
         <v>200000</v>
       </c>
     </row>
-    <row r="131" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L131" t="s">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B178" t="s">
         <v>22</v>
       </c>
-      <c r="M131" t="s">
-        <v>25</v>
-      </c>
-      <c r="N131" s="2">
+      <c r="C178" t="s">
+        <v>25</v>
+      </c>
+      <c r="D178" s="2">
         <v>60000</v>
       </c>
     </row>
-    <row r="132" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L132" t="s">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B179" t="s">
         <v>23</v>
       </c>
-      <c r="M132" t="s">
-        <v>26</v>
-      </c>
-      <c r="N132" s="2">
+      <c r="C179" t="s">
+        <v>26</v>
+      </c>
+      <c r="D179" s="2">
         <v>100000</v>
       </c>
     </row>
-    <row r="133" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L133" t="s">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B180" t="s">
         <v>24</v>
       </c>
-      <c r="M133" t="s">
-        <v>26</v>
-      </c>
-      <c r="N133" s="2">
+      <c r="C180" t="s">
+        <v>26</v>
+      </c>
+      <c r="D180" s="2">
         <v>4000000</v>
       </c>
     </row>
-    <row r="134" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L134" t="s">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B181" t="s">
         <v>28</v>
       </c>
-      <c r="M134" t="s">
-        <v>25</v>
-      </c>
-      <c r="N134" s="2">
+      <c r="C181" t="s">
+        <v>25</v>
+      </c>
+      <c r="D181" s="2">
         <v>10000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel file containing volume data.
</commit_message>
<xml_diff>
--- a/tabella dei volumi.xlsx
+++ b/tabella dei volumi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ezmirondeniku/Desktop/elaborato-database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE2ABD1-DA1B-E542-B4DA-F8EF29058CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0A4226-69CC-BB4F-A558-03F6537533E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{43723271-4DD4-433C-9C4E-C013E360E198}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="149">
   <si>
     <t>concetto</t>
   </si>
@@ -327,9 +327,6 @@
     <t>CONSULENTI</t>
   </si>
   <si>
-    <t>50000S</t>
-  </si>
-  <si>
     <t>7L</t>
   </si>
   <si>
@@ -388,13 +385,116 @@
   </si>
   <si>
     <t>100/gg</t>
+  </si>
+  <si>
+    <t>Op9b</t>
+  </si>
+  <si>
+    <t>Aggiunta recensione CVA</t>
+  </si>
+  <si>
+    <t>SERVIZIO CVA</t>
+  </si>
+  <si>
+    <t>3L</t>
+  </si>
+  <si>
+    <t>30/gg</t>
+  </si>
+  <si>
+    <t>270/gg</t>
+  </si>
+  <si>
+    <t>Aggiunta recensione INT</t>
+  </si>
+  <si>
+    <t>SERVIZIO INT</t>
+  </si>
+  <si>
+    <t>5000S</t>
+  </si>
+  <si>
+    <t>2S</t>
+  </si>
+  <si>
+    <t>500/g</t>
+  </si>
+  <si>
+    <t>4S</t>
+  </si>
+  <si>
+    <t>6L</t>
+  </si>
+  <si>
+    <t>80/gg</t>
+  </si>
+  <si>
+    <t>1120/gg</t>
+  </si>
+  <si>
+    <t>Op10</t>
+  </si>
+  <si>
+    <t>Visualizzazione dipenti in base a filtri(eta,mediarensioni)</t>
+  </si>
+  <si>
+    <t>DIPENDENTE</t>
+  </si>
+  <si>
+    <t>3000L</t>
+  </si>
+  <si>
+    <t>50/gg</t>
+  </si>
+  <si>
+    <t>150000/gg</t>
+  </si>
+  <si>
+    <t>Op11</t>
+  </si>
+  <si>
+    <t>ACQUISTO IS</t>
+  </si>
+  <si>
+    <t>Visualizzazione 10 articoli più venduti</t>
+  </si>
+  <si>
+    <t>5500000L</t>
+  </si>
+  <si>
+    <t>5500000/sett</t>
+  </si>
+  <si>
+    <t>1 settimanel</t>
+  </si>
+  <si>
+    <t>Op12</t>
+  </si>
+  <si>
+    <t>3/m</t>
+  </si>
+  <si>
+    <t>6/m</t>
+  </si>
+  <si>
+    <t>Aggiunta nuovo accessorio</t>
+  </si>
+  <si>
+    <t>Op13</t>
+  </si>
+  <si>
+    <t>Aggiunta nuovo pezzo di ricambio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +536,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -469,10 +576,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -483,8 +591,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1097,17 +1209,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7CF6F4-9A21-6746-81DA-F55FEE7F3A9F}">
-  <dimension ref="A1:AJ144"/>
+  <dimension ref="A1:AJ175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="I109" sqref="I109"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="J173" sqref="J173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1260,7 +1375,7 @@
         <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" t="s">
         <v>75</v>
@@ -1272,7 +1387,7 @@
         <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1467,7 +1582,7 @@
         <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
         <v>75</v>
@@ -1702,7 +1817,7 @@
         <v>68</v>
       </c>
       <c r="B54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C54" t="s">
         <v>75</v>
@@ -1730,7 +1845,7 @@
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AE59" s="5" t="s">
         <v>30</v>
@@ -1845,10 +1960,10 @@
         <v>2</v>
       </c>
       <c r="E64" t="s">
+        <v>105</v>
+      </c>
+      <c r="F64" t="s">
         <v>106</v>
-      </c>
-      <c r="F64" t="s">
-        <v>107</v>
       </c>
       <c r="AA64" s="7" t="s">
         <v>37</v>
@@ -2047,7 +2162,7 @@
         <v>68</v>
       </c>
       <c r="AB74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AC74" t="s">
         <v>75</v>
@@ -2198,7 +2313,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B86" t="s">
         <v>93</v>
@@ -2336,7 +2451,7 @@
         <v>90</v>
       </c>
       <c r="B96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>75</v>
@@ -2348,12 +2463,12 @@
         <v>92</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B100" t="s">
         <v>94</v>
@@ -2486,7 +2601,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="B110" t="s">
         <v>91</v>
@@ -2501,15 +2616,15 @@
         <v>92</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>111</v>
+      </c>
+      <c r="B114" t="s">
         <v>112</v>
-      </c>
-      <c r="B114" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:17" ht="16" x14ac:dyDescent="0.2">
@@ -2528,7 +2643,7 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B116" t="s">
         <v>25</v>
@@ -2542,7 +2657,7 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B117" t="s">
         <v>26</v>
@@ -2556,7 +2671,7 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B118" t="s">
         <v>25</v>
@@ -2583,7 +2698,7 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B120" t="s">
         <v>83</v>
@@ -2592,13 +2707,13 @@
         <v>75</v>
       </c>
       <c r="D120" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="M120" s="1" t="s">
         <v>0</v>
@@ -2633,6 +2748,12 @@
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>116</v>
+      </c>
+      <c r="B123" t="s">
+        <v>117</v>
+      </c>
       <c r="M123" t="s">
         <v>5</v>
       </c>
@@ -2645,7 +2766,19 @@
       <c r="P123" s="7"/>
       <c r="Q123" s="7"/>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="M124" t="s">
         <v>6</v>
       </c>
@@ -2659,6 +2792,18 @@
       <c r="Q124" s="7"/>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>109</v>
+      </c>
+      <c r="B125" t="s">
+        <v>25</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+      <c r="D125" t="s">
+        <v>41</v>
+      </c>
       <c r="M125" t="s">
         <v>7</v>
       </c>
@@ -2670,6 +2815,18 @@
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>110</v>
+      </c>
+      <c r="B126" t="s">
+        <v>26</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+      <c r="D126" t="s">
+        <v>41</v>
+      </c>
       <c r="M126" t="s">
         <v>8</v>
       </c>
@@ -2681,6 +2838,18 @@
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>118</v>
+      </c>
+      <c r="B127" t="s">
+        <v>25</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127" t="s">
+        <v>42</v>
+      </c>
       <c r="M127" t="s">
         <v>9</v>
       </c>
@@ -2692,6 +2861,18 @@
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>50</v>
+      </c>
+      <c r="B128" t="s">
+        <v>26</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128" t="s">
+        <v>42</v>
+      </c>
       <c r="M128" t="s">
         <v>10</v>
       </c>
@@ -2702,7 +2883,19 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="129" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>51</v>
+      </c>
+      <c r="B129" t="s">
+        <v>25</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129" t="s">
+        <v>42</v>
+      </c>
       <c r="M129" t="s">
         <v>11</v>
       </c>
@@ -2713,7 +2906,19 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="130" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>51</v>
+      </c>
+      <c r="B130" t="s">
+        <v>25</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130" t="s">
+        <v>41</v>
+      </c>
       <c r="M130" t="s">
         <v>27</v>
       </c>
@@ -2724,7 +2929,18 @@
         <v>2500000</v>
       </c>
     </row>
-    <row r="131" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A131" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C131" s="7"/>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="M131" t="s">
         <v>12</v>
       </c>
@@ -2735,7 +2951,25 @@
         <v>2500000</v>
       </c>
     </row>
-    <row r="132" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>114</v>
+      </c>
+      <c r="B132" t="s">
+        <v>119</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D132" s="7">
+        <v>9</v>
+      </c>
+      <c r="E132" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F132" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="M132" t="s">
         <v>13</v>
       </c>
@@ -2746,7 +2980,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="133" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M133" t="s">
         <v>14</v>
       </c>
@@ -2757,7 +2991,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="134" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M134" t="s">
         <v>15</v>
       </c>
@@ -2768,7 +3002,13 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="135" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>116</v>
+      </c>
+      <c r="B135" t="s">
+        <v>122</v>
+      </c>
       <c r="M135" t="s">
         <v>16</v>
       </c>
@@ -2779,7 +3019,19 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="136" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A136" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="M136" t="s">
         <v>17</v>
       </c>
@@ -2790,7 +3042,19 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="137" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>109</v>
+      </c>
+      <c r="B137" t="s">
+        <v>25</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="D137" t="s">
+        <v>41</v>
+      </c>
       <c r="M137" t="s">
         <v>18</v>
       </c>
@@ -2801,7 +3065,19 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="138" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>110</v>
+      </c>
+      <c r="B138" t="s">
+        <v>26</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+      <c r="D138" t="s">
+        <v>41</v>
+      </c>
       <c r="M138" t="s">
         <v>19</v>
       </c>
@@ -2812,7 +3088,19 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="139" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>123</v>
+      </c>
+      <c r="B139" t="s">
+        <v>25</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139" t="s">
+        <v>42</v>
+      </c>
       <c r="M139" t="s">
         <v>20</v>
       </c>
@@ -2823,7 +3111,19 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="140" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>58</v>
+      </c>
+      <c r="B140" t="s">
+        <v>26</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+      <c r="D140" t="s">
+        <v>42</v>
+      </c>
       <c r="M140" t="s">
         <v>21</v>
       </c>
@@ -2834,7 +3134,19 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="141" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>59</v>
+      </c>
+      <c r="B141" t="s">
+        <v>25</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141" t="s">
+        <v>42</v>
+      </c>
       <c r="M141" t="s">
         <v>22</v>
       </c>
@@ -2845,7 +3157,19 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="142" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>59</v>
+      </c>
+      <c r="B142" t="s">
+        <v>25</v>
+      </c>
+      <c r="C142">
+        <v>2</v>
+      </c>
+      <c r="D142" t="s">
+        <v>41</v>
+      </c>
       <c r="M142" t="s">
         <v>23</v>
       </c>
@@ -2856,7 +3180,18 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="143" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A143" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C143" s="7"/>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F143" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="M143" t="s">
         <v>24</v>
       </c>
@@ -2867,7 +3202,25 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="144" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>127</v>
+      </c>
+      <c r="B144" t="s">
+        <v>128</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D144" s="7">
+        <v>14</v>
+      </c>
+      <c r="E144" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F144" s="7" t="s">
+        <v>130</v>
+      </c>
       <c r="M144" t="s">
         <v>28</v>
       </c>
@@ -2876,6 +3229,298 @@
       </c>
       <c r="O144" s="2">
         <v>10000000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>131</v>
+      </c>
+      <c r="B147" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A148" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>133</v>
+      </c>
+      <c r="B149" t="s">
+        <v>25</v>
+      </c>
+      <c r="C149">
+        <v>3000</v>
+      </c>
+      <c r="D149" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A150" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C150" s="7"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F150" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B151" t="s">
+        <v>134</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D151" s="7">
+        <v>3000</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F151" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>137</v>
+      </c>
+      <c r="B154" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A155" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>138</v>
+      </c>
+      <c r="B156" t="s">
+        <v>25</v>
+      </c>
+      <c r="C156">
+        <v>500000</v>
+      </c>
+      <c r="D156" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>39</v>
+      </c>
+      <c r="B157" t="s">
+        <v>26</v>
+      </c>
+      <c r="C157" s="9">
+        <v>2500000</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>40</v>
+      </c>
+      <c r="B158" t="s">
+        <v>25</v>
+      </c>
+      <c r="C158" s="10">
+        <v>2500000</v>
+      </c>
+      <c r="D158" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A159" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C159" s="7"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F159" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B160" t="s">
+        <v>140</v>
+      </c>
+      <c r="C160" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D160" s="7">
+        <v>5500000</v>
+      </c>
+      <c r="E160" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F160" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>143</v>
+      </c>
+      <c r="B164" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A165" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D165" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>40</v>
+      </c>
+      <c r="B166" t="s">
+        <v>25</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="D166" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A167" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C167" s="7"/>
+      <c r="D167" s="7"/>
+      <c r="E167" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F167" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>67</v>
+      </c>
+      <c r="C168" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D168" s="7">
+        <v>2</v>
+      </c>
+      <c r="E168" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F168" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>147</v>
+      </c>
+      <c r="B171" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A172" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>62</v>
+      </c>
+      <c r="B173" t="s">
+        <v>25</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+      <c r="D173" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A174" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C174" s="7"/>
+      <c r="D174" s="7"/>
+      <c r="E174" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F174" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>67</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D175" s="7">
+        <v>2</v>
+      </c>
+      <c r="E175" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="F175" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>